<commit_message>
minor changes (if any)
</commit_message>
<xml_diff>
--- a/data/data_2024-01-22_LSR3_H.xlsx
+++ b/data/data_2024-01-22_LSR3_H.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EA26"/>
+  <dimension ref="A1:EC26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1013,6 +1013,16 @@
           <t>qtc_md_se</t>
         </is>
       </c>
+      <c r="EB1" s="1" t="inlineStr">
+        <is>
+          <t>study_name_drug</t>
+        </is>
+      </c>
+      <c r="EC1" s="1" t="inlineStr">
+        <is>
+          <t>crossover_periods</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1290,6 +1300,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB2" t="inlineStr">
+        <is>
+          <t>Isaacson (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1585,6 +1603,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB3" t="inlineStr">
+        <is>
+          <t>Isaacson (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1999,6 +2025,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB4" t="inlineStr">
+        <is>
+          <t>Koblan (2020) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2413,6 +2447,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB5" t="inlineStr">
+        <is>
+          <t>Koblan (2020) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2566,6 +2608,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB6" t="inlineStr">
+        <is>
+          <t>NCT04072354 (2019) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2719,6 +2769,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB7" t="inlineStr">
+        <is>
+          <t>NCT04072354 (2019) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2872,6 +2930,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB8" t="inlineStr">
+        <is>
+          <t>NCT04072354 (2019) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3025,6 +3091,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB9" t="inlineStr">
+        <is>
+          <t>NCT04092686 (2019) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3178,6 +3252,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB10" t="inlineStr">
+        <is>
+          <t>NCT04092686 (2019) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3331,6 +3413,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB11" t="inlineStr">
+        <is>
+          <t>NCT04092686 (2019) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3655,6 +3745,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB12" t="inlineStr">
+        <is>
+          <t>NCT04512066 (2020) - ralmitaront</t>
+        </is>
+      </c>
+      <c r="EC12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3979,6 +4077,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB13" t="inlineStr">
+        <is>
+          <t>NCT04512066 (2020) - ralmitaront</t>
+        </is>
+      </c>
+      <c r="EC13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -4303,6 +4409,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB14" t="inlineStr">
+        <is>
+          <t>NCT04512066 (2020) - ralmitaront</t>
+        </is>
+      </c>
+      <c r="EC14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -4627,6 +4741,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB15" t="inlineStr">
+        <is>
+          <t>NCT04512066 (2020) - ralmitaront</t>
+        </is>
+      </c>
+      <c r="EC15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -4778,6 +4900,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB16" t="inlineStr">
+        <is>
+          <t>Perini (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -4929,6 +5059,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB17" t="inlineStr">
+        <is>
+          <t>Perini (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -5080,6 +5218,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB18" t="inlineStr">
+        <is>
+          <t>Perini (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -5214,6 +5360,14 @@
       <c r="EA19">
         <v>2.100625000000001</v>
       </c>
+      <c r="EB19" t="inlineStr">
+        <is>
+          <t>Tsukada (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -5364,6 +5518,14 @@
       <c r="EA20">
         <v>2.100625000000001</v>
       </c>
+      <c r="EB20" t="inlineStr">
+        <is>
+          <t>Tsukada (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC20">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5503,6 +5665,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB21" t="inlineStr">
+        <is>
+          <t>Hopkins (2021) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC21">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5642,6 +5812,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB22" t="inlineStr">
+        <is>
+          <t>Hopkins (2021) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC22">
+        <v>2</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5781,6 +5959,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB23" t="inlineStr">
+        <is>
+          <t>Hopkins (2021) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC23">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -5876,6 +6062,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB24" t="inlineStr">
+        <is>
+          <t>Szabo (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC24">
+        <v>3</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5971,6 +6165,14 @@
           <t>yes</t>
         </is>
       </c>
+      <c r="EB25" t="inlineStr">
+        <is>
+          <t>Szabo (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC25">
+        <v>3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -6065,6 +6267,14 @@
         <is>
           <t>yes</t>
         </is>
+      </c>
+      <c r="EB26" t="inlineStr">
+        <is>
+          <t>Szabo (2023) - ulotaront</t>
+        </is>
+      </c>
+      <c r="EC26">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>